<commit_message>
created the system for storing workouts. Will soon also be able to print workouts from their storage
</commit_message>
<xml_diff>
--- a/backend/data/raw/workouts_to_database.xlsx
+++ b/backend/data/raw/workouts_to_database.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29016"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D6E93AA-1936-4FE0-9235-EDF6521DFB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48f10a2996282021/Desktop/AI-Training-Plan/AI-Training-Plans/backend/data/raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1498450E-0511-4CEC-A2FE-6553D84431D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC0DB6FB-2978-4284-84C2-E35A7C82E4B5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="10008" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,29 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Workout:</t>
-  </si>
-  <si>
-    <t>(Stim, RPE, Dist)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Reps</t>
   </si>
@@ -48,20 +36,32 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>(1,2,3)</t>
-  </si>
-  <si>
-    <t>(1,1)</t>
-  </si>
-  <si>
     <t>5000 3000</t>
+  </si>
+  <si>
+    <t>5000 5000</t>
+  </si>
+  <si>
+    <t>2, 2</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>1, 2, 3</t>
+  </si>
+  <si>
+    <t>4, 5, 6</t>
+  </si>
+  <si>
+    <t>Trio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,48 +427,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>50</v>
+      <c r="D3">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doesn't matter its gonna be overwritten
</commit_message>
<xml_diff>
--- a/backend/data/raw/workouts_to_database.xlsx
+++ b/backend/data/raw/workouts_to_database.xlsx
@@ -120,6 +120,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,7 +447,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
workouts are now functional with float inputs in the trio
</commit_message>
<xml_diff>
--- a/backend/data/raw/workouts_to_database.xlsx
+++ b/backend/data/raw/workouts_to_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48f10a2996282021/Desktop/AI-Training-Plan/AI-Training-Plans/backend/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{910D3C3D-05A1-4061-BAB6-7FBFD98D6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{868BEE6F-C50A-4C1D-B20E-7C78439F430A}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{910D3C3D-05A1-4061-BAB6-7FBFD98D6AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A110345-648B-482D-8A35-C8BAA729589F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Reps</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>4, 5, 7</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>2.5, 4, 5.5</t>
+  </si>
+  <si>
+    <t>2.5, 4, 4,5</t>
+  </si>
+  <si>
+    <t>2.5, 4, 5</t>
   </si>
 </sst>
 </file>
@@ -446,11 +458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,6 +541,48 @@
         <v>80</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>